<commit_message>
final version of the project- implements bloom filters, uses heaps and priority queues correctly, implementation of map is fixed fully and the data reading and writing to files is accurate
</commit_message>
<xml_diff>
--- a/map.xlsx
+++ b/map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asma/Desktop/📎/nust/sophmore/data structure + algorithms/project/ride-sharing-system/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FEFE94D-43BA-A049-823A-E2AC0BD6D29D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8552CD-BECB-E74B-BF4A-D98E92F646F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{37E5F4C1-E943-F84A-B791-66CC2F3CEE04}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{37E5F4C1-E943-F84A-B791-66CC2F3CEE04}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>housing complex a</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>public hospital, private hospital</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -196,7 +199,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -206,6 +209,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -412,87 +421,81 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -809,10 +812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E61C1AC-9909-5445-9D26-4C8B0834513C}">
-  <dimension ref="A1:W40"/>
+  <dimension ref="A1:U40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V18" sqref="V18"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="116" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B40" sqref="B23:N40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -835,656 +838,615 @@
     <col min="21" max="21" width="3.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5">
+    <row r="1" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4">
         <v>20</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="67"/>
-    </row>
-    <row r="2" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
+      <c r="P1" s="60"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="60"/>
+      <c r="S1" s="60"/>
+      <c r="T1" s="60"/>
+      <c r="U1" s="61"/>
+    </row>
+    <row r="2" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
         <v>19</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="49" t="s">
+      <c r="B2" s="34"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="68"/>
+      <c r="P2" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="Q2" s="46"/>
-      <c r="R2" s="50"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="47" t="s">
+      <c r="Q2" s="68"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="63"/>
+      <c r="T2" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="U2" s="9"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-    </row>
-    <row r="3" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
+      <c r="U2" s="65"/>
+    </row>
+    <row r="3" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
         <v>18</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="9"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-    </row>
-    <row r="4" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
+      <c r="B3" s="62"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="66"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="66"/>
+      <c r="M3" s="63"/>
+      <c r="N3" s="66"/>
+      <c r="O3" s="63"/>
+      <c r="P3" s="63"/>
+      <c r="Q3" s="63"/>
+      <c r="R3" s="63"/>
+      <c r="S3" s="63"/>
+      <c r="T3" s="66"/>
+      <c r="U3" s="65"/>
+    </row>
+    <row r="4" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
         <v>17</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="56"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="44"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="32"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="58" t="s">
+      <c r="C4" s="63"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="63"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="63"/>
+      <c r="N4" s="24"/>
+      <c r="O4" s="63"/>
+      <c r="P4" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="61"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="48"/>
-      <c r="U4" s="9"/>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
-    </row>
-    <row r="5" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
+      <c r="Q4" s="60"/>
+      <c r="R4" s="51"/>
+      <c r="S4" s="63"/>
+      <c r="T4" s="38"/>
+      <c r="U4" s="65"/>
+    </row>
+    <row r="5" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
         <v>16</v>
       </c>
-      <c r="B5" s="43"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="25"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="9"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="9"/>
-      <c r="V5" s="2"/>
-      <c r="W5" s="2"/>
-    </row>
-    <row r="6" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
+      <c r="B5" s="62"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="66"/>
+      <c r="K5" s="63"/>
+      <c r="L5" s="66"/>
+      <c r="M5" s="63"/>
+      <c r="N5" s="66"/>
+      <c r="O5" s="63"/>
+      <c r="P5" s="64"/>
+      <c r="Q5" s="63"/>
+      <c r="R5" s="65"/>
+      <c r="S5" s="63"/>
+      <c r="T5" s="63"/>
+      <c r="U5" s="65"/>
+    </row>
+    <row r="6" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
         <v>15</v>
       </c>
-      <c r="B6" s="52"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="21" t="s">
+      <c r="B6" s="42"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="56"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="44"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="45"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="59"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="60"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="39"/>
-      <c r="U6" s="9"/>
-      <c r="V6" s="2"/>
-      <c r="W6" s="2"/>
-    </row>
-    <row r="7" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
+      <c r="G6" s="63"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="63"/>
+      <c r="L6" s="35"/>
+      <c r="M6" s="63"/>
+      <c r="N6" s="36"/>
+      <c r="O6" s="63"/>
+      <c r="P6" s="49"/>
+      <c r="Q6" s="67"/>
+      <c r="R6" s="50"/>
+      <c r="S6" s="63"/>
+      <c r="T6" s="31"/>
+      <c r="U6" s="65"/>
+    </row>
+    <row r="7" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
         <v>14</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="25"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="8"/>
-      <c r="T7" s="25"/>
-      <c r="U7" s="9"/>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A8" s="10">
+      <c r="B7" s="63"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="63"/>
+      <c r="J7" s="66"/>
+      <c r="K7" s="63"/>
+      <c r="L7" s="66"/>
+      <c r="M7" s="63"/>
+      <c r="N7" s="63"/>
+      <c r="O7" s="63"/>
+      <c r="P7" s="63"/>
+      <c r="Q7" s="63"/>
+      <c r="R7" s="63"/>
+      <c r="S7" s="63"/>
+      <c r="T7" s="66"/>
+      <c r="U7" s="65"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
         <v>13</v>
       </c>
-      <c r="B8" s="47"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="56" t="s">
+      <c r="B8" s="37"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="63"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="63"/>
+      <c r="J8" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="K8" s="8"/>
-      <c r="L8" s="44"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="20"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="23"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="40" t="s">
+      <c r="K8" s="63"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="63"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="60"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="60"/>
+      <c r="R8" s="16"/>
+      <c r="S8" s="63"/>
+      <c r="T8" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="U8" s="9"/>
-      <c r="V8" s="2"/>
-      <c r="W8" s="2"/>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A9" s="10">
+      <c r="U8" s="65"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
         <v>12</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="25"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="9"/>
-      <c r="S9" s="8"/>
-      <c r="T9" s="25"/>
-      <c r="U9" s="9"/>
-      <c r="V9" s="2"/>
-      <c r="W9" s="2"/>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A10" s="10">
+      <c r="B9" s="66"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="63"/>
+      <c r="H9" s="65"/>
+      <c r="I9" s="63"/>
+      <c r="J9" s="66"/>
+      <c r="K9" s="63"/>
+      <c r="L9" s="66"/>
+      <c r="M9" s="63"/>
+      <c r="N9" s="64"/>
+      <c r="O9" s="63"/>
+      <c r="P9" s="63"/>
+      <c r="Q9" s="63"/>
+      <c r="R9" s="65"/>
+      <c r="S9" s="63"/>
+      <c r="T9" s="66"/>
+      <c r="U9" s="65"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
         <v>11</v>
       </c>
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="56"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="44" t="s">
+      <c r="C10" s="63"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="63"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="63"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="63"/>
+      <c r="L10" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="M10" s="8"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="22"/>
-      <c r="S10" s="8"/>
-      <c r="T10" s="40"/>
-      <c r="U10" s="9"/>
-      <c r="V10" s="2"/>
-      <c r="W10" s="2"/>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A11" s="10">
+      <c r="M10" s="63"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="63"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="63"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="63"/>
+      <c r="T10" s="32"/>
+      <c r="U10" s="65"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
         <v>10</v>
       </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="8"/>
-      <c r="R11" s="9"/>
-      <c r="S11" s="8"/>
-      <c r="T11" s="25"/>
-      <c r="U11" s="9"/>
-      <c r="V11" s="2"/>
-      <c r="W11" s="2"/>
-    </row>
-    <row r="12" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10">
+      <c r="B11" s="66"/>
+      <c r="C11" s="63"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="65"/>
+      <c r="I11" s="63"/>
+      <c r="J11" s="66"/>
+      <c r="K11" s="63"/>
+      <c r="L11" s="66"/>
+      <c r="M11" s="63"/>
+      <c r="N11" s="64"/>
+      <c r="O11" s="63"/>
+      <c r="P11" s="63"/>
+      <c r="Q11" s="63"/>
+      <c r="R11" s="65"/>
+      <c r="S11" s="63"/>
+      <c r="T11" s="66"/>
+      <c r="U11" s="65"/>
+    </row>
+    <row r="12" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
         <v>9</v>
       </c>
-      <c r="B12" s="44"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="57"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="48"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="19"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="22"/>
-      <c r="S12" s="8"/>
-      <c r="T12" s="40"/>
-      <c r="U12" s="9"/>
-      <c r="V12" s="2"/>
-      <c r="W12" s="2"/>
-    </row>
-    <row r="13" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10">
+      <c r="B12" s="35"/>
+      <c r="C12" s="63"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="67"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="63"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="63"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="63"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="63"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="63"/>
+      <c r="R12" s="15"/>
+      <c r="S12" s="63"/>
+      <c r="T12" s="32"/>
+      <c r="U12" s="65"/>
+    </row>
+    <row r="13" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
         <v>8</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="9"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="25"/>
-      <c r="U13" s="9"/>
-      <c r="V13" s="2"/>
-      <c r="W13" s="2"/>
-    </row>
-    <row r="14" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10">
+      <c r="B13" s="66"/>
+      <c r="C13" s="63"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="63"/>
+      <c r="I13" s="63"/>
+      <c r="J13" s="63"/>
+      <c r="K13" s="63"/>
+      <c r="L13" s="63"/>
+      <c r="M13" s="63"/>
+      <c r="N13" s="64"/>
+      <c r="O13" s="63"/>
+      <c r="P13" s="63"/>
+      <c r="Q13" s="63"/>
+      <c r="R13" s="65"/>
+      <c r="S13" s="63"/>
+      <c r="T13" s="66"/>
+      <c r="U13" s="65"/>
+    </row>
+    <row r="14" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
         <v>7</v>
       </c>
-      <c r="B14" s="48"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="66"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="54"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="33"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="38"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="21" t="s">
+      <c r="B14" s="38"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="63"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="63"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="60"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="63"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="63"/>
+      <c r="P14" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="Q14" s="8"/>
-      <c r="R14" s="22"/>
-      <c r="S14" s="8"/>
-      <c r="T14" s="40"/>
-      <c r="U14" s="9"/>
-      <c r="V14" s="2"/>
-      <c r="W14" s="2"/>
-    </row>
-    <row r="15" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10">
+      <c r="Q14" s="63"/>
+      <c r="R14" s="15"/>
+      <c r="S14" s="63"/>
+      <c r="T14" s="32"/>
+      <c r="U14" s="65"/>
+    </row>
+    <row r="15" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
         <v>6</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="8"/>
-      <c r="R15" s="9"/>
-      <c r="S15" s="8"/>
-      <c r="T15" s="25"/>
-      <c r="U15" s="9"/>
-      <c r="V15" s="2"/>
-      <c r="W15" s="2"/>
-    </row>
-    <row r="16" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10">
+      <c r="B15" s="63"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="66"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="66"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="64"/>
+      <c r="K15" s="63"/>
+      <c r="L15" s="65"/>
+      <c r="M15" s="63"/>
+      <c r="N15" s="64"/>
+      <c r="O15" s="63"/>
+      <c r="P15" s="63"/>
+      <c r="Q15" s="63"/>
+      <c r="R15" s="65"/>
+      <c r="S15" s="63"/>
+      <c r="T15" s="66"/>
+      <c r="U15" s="65"/>
+    </row>
+    <row r="16" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
         <v>5</v>
       </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="32" t="s">
+      <c r="B16" s="25"/>
+      <c r="C16" s="60"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="63"/>
+      <c r="F16" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="53" t="s">
+      <c r="G16" s="63"/>
+      <c r="H16" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I16" s="8"/>
-      <c r="J16" s="34" t="s">
+      <c r="I16" s="63"/>
+      <c r="J16" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="K16" s="8"/>
-      <c r="L16" s="37"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="17"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="19"/>
-      <c r="Q16" s="8"/>
-      <c r="R16" s="22"/>
-      <c r="S16" s="8"/>
-      <c r="T16" s="65"/>
-      <c r="U16" s="9"/>
-      <c r="V16" s="2"/>
-      <c r="W16" s="2"/>
-    </row>
-    <row r="17" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10">
+      <c r="K16" s="63"/>
+      <c r="L16" s="29"/>
+      <c r="M16" s="63"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="63"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="63"/>
+      <c r="R16" s="15"/>
+      <c r="S16" s="63"/>
+      <c r="T16" s="55"/>
+      <c r="U16" s="65"/>
+    </row>
+    <row r="17" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
         <v>4</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="8"/>
-      <c r="P17" s="8"/>
-      <c r="Q17" s="8"/>
-      <c r="R17" s="9"/>
-      <c r="S17" s="8"/>
-      <c r="T17" s="8"/>
-      <c r="U17" s="9"/>
-      <c r="V17" s="2"/>
-      <c r="W17" s="2"/>
-    </row>
-    <row r="18" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
+      <c r="B17" s="64"/>
+      <c r="C17" s="63"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="63"/>
+      <c r="F17" s="66"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="63"/>
+      <c r="I17" s="63"/>
+      <c r="J17" s="64"/>
+      <c r="K17" s="63"/>
+      <c r="L17" s="65"/>
+      <c r="M17" s="63"/>
+      <c r="N17" s="64"/>
+      <c r="O17" s="63"/>
+      <c r="P17" s="63"/>
+      <c r="Q17" s="63"/>
+      <c r="R17" s="65"/>
+      <c r="S17" s="63"/>
+      <c r="T17" s="63"/>
+      <c r="U17" s="65"/>
+    </row>
+    <row r="18" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
         <v>3</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="34"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="37"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="17"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="18"/>
-      <c r="Q18" s="13"/>
-      <c r="R18" s="24"/>
-      <c r="S18" s="8"/>
-      <c r="T18" s="54"/>
-      <c r="U18" s="9"/>
-      <c r="V18" s="2"/>
-      <c r="W18" s="2"/>
-    </row>
-    <row r="19" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="10">
+      <c r="C18" s="63"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="63"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="63"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="63"/>
+      <c r="L18" s="29"/>
+      <c r="M18" s="63"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="67"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="67"/>
+      <c r="R18" s="17"/>
+      <c r="S18" s="63"/>
+      <c r="T18" s="44"/>
+      <c r="U18" s="65"/>
+    </row>
+    <row r="19" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
         <v>2</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="25"/>
-      <c r="O19" s="8"/>
-      <c r="P19" s="8"/>
-      <c r="Q19" s="8"/>
-      <c r="R19" s="8"/>
-      <c r="S19" s="8"/>
-      <c r="T19" s="25"/>
-      <c r="U19" s="9"/>
-      <c r="V19" s="2"/>
-      <c r="W19" s="2"/>
-    </row>
-    <row r="20" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="10">
+      <c r="B19" s="64"/>
+      <c r="C19" s="63"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="63"/>
+      <c r="F19" s="64"/>
+      <c r="G19" s="63"/>
+      <c r="H19" s="65"/>
+      <c r="I19" s="63"/>
+      <c r="J19" s="64"/>
+      <c r="K19" s="63"/>
+      <c r="L19" s="65"/>
+      <c r="M19" s="63"/>
+      <c r="N19" s="66"/>
+      <c r="O19" s="63"/>
+      <c r="P19" s="63"/>
+      <c r="Q19" s="63"/>
+      <c r="R19" s="63"/>
+      <c r="S19" s="63"/>
+      <c r="T19" s="66"/>
+      <c r="U19" s="65"/>
+    </row>
+    <row r="20" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
         <v>1</v>
       </c>
-      <c r="B20" s="35"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="35"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="36"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="66"/>
-      <c r="O20" s="8"/>
-      <c r="P20" s="63"/>
-      <c r="Q20" s="46"/>
-      <c r="R20" s="64"/>
-      <c r="S20" s="46"/>
-      <c r="T20" s="72" t="s">
+      <c r="B20" s="27"/>
+      <c r="C20" s="67"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="63"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="67"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="63"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="67"/>
+      <c r="L20" s="28"/>
+      <c r="M20" s="63"/>
+      <c r="N20" s="56"/>
+      <c r="O20" s="63"/>
+      <c r="P20" s="53"/>
+      <c r="Q20" s="68"/>
+      <c r="R20" s="54"/>
+      <c r="S20" s="68"/>
+      <c r="T20" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="U20" s="9"/>
-      <c r="V20" s="2"/>
-      <c r="W20" s="2"/>
-    </row>
-    <row r="21" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
-      <c r="B21" s="14">
+      <c r="U20" s="65"/>
+    </row>
+    <row r="21" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="7">
         <v>1</v>
       </c>
-      <c r="C21" s="14">
+      <c r="C21" s="7">
         <v>2</v>
       </c>
-      <c r="D21" s="14">
+      <c r="D21" s="7">
         <v>3</v>
       </c>
-      <c r="E21" s="14">
+      <c r="E21" s="7">
         <v>4</v>
       </c>
-      <c r="F21" s="14">
+      <c r="F21" s="7">
         <v>5</v>
       </c>
-      <c r="G21" s="14">
+      <c r="G21" s="7">
         <v>6</v>
       </c>
-      <c r="H21" s="14">
+      <c r="H21" s="7">
         <v>7</v>
       </c>
-      <c r="I21" s="14">
+      <c r="I21" s="7">
         <v>8</v>
       </c>
-      <c r="J21" s="14">
+      <c r="J21" s="7">
         <v>9</v>
       </c>
-      <c r="K21" s="14">
+      <c r="K21" s="7">
         <v>10</v>
       </c>
-      <c r="L21" s="14">
+      <c r="L21" s="7">
         <v>11</v>
       </c>
-      <c r="M21" s="14">
+      <c r="M21" s="7">
         <v>12</v>
       </c>
-      <c r="N21" s="14">
+      <c r="N21" s="7">
         <v>13</v>
       </c>
-      <c r="O21" s="14">
+      <c r="O21" s="7">
         <v>14</v>
       </c>
-      <c r="P21" s="14">
+      <c r="P21" s="7">
         <v>15</v>
       </c>
-      <c r="Q21" s="14">
+      <c r="Q21" s="7">
         <v>16</v>
       </c>
-      <c r="R21" s="14">
+      <c r="R21" s="7">
         <v>17</v>
       </c>
-      <c r="S21" s="14">
+      <c r="S21" s="7">
         <v>18</v>
       </c>
-      <c r="T21" s="14">
+      <c r="T21" s="7">
         <v>19</v>
       </c>
-      <c r="U21" s="15">
+      <c r="U21" s="8">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>13</v>
       </c>
-      <c r="T23" s="11"/>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>14</v>
       </c>
-      <c r="J24" s="11"/>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="J25" s="11"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="P25" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B26" s="69" t="s">
         <v>15</v>
       </c>
@@ -1500,12 +1462,12 @@
       <c r="L26" s="69"/>
       <c r="M26" s="69"/>
       <c r="N26" s="69"/>
-      <c r="O26" s="68"/>
+      <c r="O26" s="57"/>
       <c r="P26" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B27" s="69" t="s">
         <v>16</v>
       </c>
@@ -1521,15 +1483,15 @@
       <c r="L27" s="69"/>
       <c r="M27" s="69"/>
       <c r="N27" s="69"/>
-      <c r="O27" s="68"/>
-      <c r="P27" s="3" t="s">
+      <c r="O27" s="57"/>
+      <c r="P27" s="2" t="s">
         <v>34</v>
       </c>
       <c r="Q27" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B28" s="69" t="s">
         <v>17</v>
       </c>
@@ -1545,14 +1507,14 @@
       <c r="L28" s="69"/>
       <c r="M28" s="69"/>
       <c r="N28" s="69"/>
-      <c r="P28" s="4" t="s">
+      <c r="P28" s="3" t="s">
         <v>35</v>
       </c>
       <c r="Q28" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B29" s="69" t="s">
         <v>26</v>
       </c>
@@ -1568,14 +1530,14 @@
       <c r="L29" s="69"/>
       <c r="M29" s="69"/>
       <c r="N29" s="69"/>
-      <c r="P29" s="41" t="s">
+      <c r="P29" s="33" t="s">
         <v>37</v>
       </c>
       <c r="Q29" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B30" s="69" t="s">
         <v>18</v>
       </c>
@@ -1591,14 +1553,14 @@
       <c r="L30" s="69"/>
       <c r="M30" s="69"/>
       <c r="N30" s="69"/>
-      <c r="P30" s="62" t="s">
+      <c r="P30" s="52" t="s">
         <v>36</v>
       </c>
       <c r="Q30" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B31" s="69" t="s">
         <v>19</v>
       </c>
@@ -1614,37 +1576,37 @@
       <c r="L31" s="69"/>
       <c r="M31" s="69"/>
       <c r="N31" s="69"/>
-      <c r="P31" s="70" t="s">
+      <c r="P31" s="12" t="s">
         <v>38</v>
       </c>
       <c r="Q31" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="B32" s="73" t="s">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B32" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="73"/>
-      <c r="D32" s="73"/>
-      <c r="E32" s="73"/>
-      <c r="F32" s="73"/>
-      <c r="G32" s="73"/>
-      <c r="H32" s="73"/>
-      <c r="I32" s="73"/>
-      <c r="J32" s="73"/>
-      <c r="K32" s="73"/>
-      <c r="L32" s="73"/>
-      <c r="M32" s="73"/>
-      <c r="N32" s="73"/>
-      <c r="P32" s="71" t="s">
+      <c r="C32" s="69"/>
+      <c r="D32" s="69"/>
+      <c r="E32" s="69"/>
+      <c r="F32" s="69"/>
+      <c r="G32" s="69"/>
+      <c r="H32" s="69"/>
+      <c r="I32" s="69"/>
+      <c r="J32" s="69"/>
+      <c r="K32" s="69"/>
+      <c r="L32" s="69"/>
+      <c r="M32" s="69"/>
+      <c r="N32" s="69"/>
+      <c r="P32" s="58" t="s">
         <v>2</v>
       </c>
       <c r="Q32" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B33" s="69" t="s">
         <v>23</v>
       </c>
@@ -1661,7 +1623,7 @@
       <c r="M33" s="69"/>
       <c r="N33" s="69"/>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B34" s="69" t="s">
         <v>24</v>
       </c>
@@ -1678,7 +1640,7 @@
       <c r="M34" s="69"/>
       <c r="N34" s="69"/>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B35" s="69" t="s">
         <v>25</v>
       </c>
@@ -1695,7 +1657,7 @@
       <c r="M35" s="69"/>
       <c r="N35" s="69"/>
     </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B36" s="69" t="s">
         <v>28</v>
       </c>
@@ -1712,7 +1674,7 @@
       <c r="M36" s="69"/>
       <c r="N36" s="69"/>
     </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B37" s="69" t="s">
         <v>27</v>
       </c>
@@ -1729,7 +1691,7 @@
       <c r="M37" s="69"/>
       <c r="N37" s="69"/>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B38" s="69" t="s">
         <v>29</v>
       </c>
@@ -1746,7 +1708,7 @@
       <c r="M38" s="69"/>
       <c r="N38" s="69"/>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B39" s="69" t="s">
         <v>31</v>
       </c>
@@ -1762,8 +1724,11 @@
       <c r="L39" s="69"/>
       <c r="M39" s="69"/>
       <c r="N39" s="69"/>
-    </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="P39" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B40" s="69" t="s">
         <v>32</v>
       </c>
@@ -1782,6 +1747,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B40:N40"/>
+    <mergeCell ref="B28:N28"/>
+    <mergeCell ref="B39:N39"/>
+    <mergeCell ref="B38:N38"/>
+    <mergeCell ref="B37:N37"/>
+    <mergeCell ref="B36:N36"/>
+    <mergeCell ref="B35:N35"/>
     <mergeCell ref="B26:N26"/>
     <mergeCell ref="B27:N27"/>
     <mergeCell ref="B34:N34"/>
@@ -1790,13 +1762,6 @@
     <mergeCell ref="B31:N31"/>
     <mergeCell ref="B30:N30"/>
     <mergeCell ref="B29:N29"/>
-    <mergeCell ref="B40:N40"/>
-    <mergeCell ref="B28:N28"/>
-    <mergeCell ref="B39:N39"/>
-    <mergeCell ref="B38:N38"/>
-    <mergeCell ref="B37:N37"/>
-    <mergeCell ref="B36:N36"/>
-    <mergeCell ref="B35:N35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>